<commit_message>
update Bao Cao va Testcase
</commit_message>
<xml_diff>
--- a/Testcase.xlsx
+++ b/Testcase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hk3-nam3\CNPM-NC\LT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hk3-nam3\CNPM-NC\LT\Nhom2_QLKTX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D7D30A-5339-4493-BDE5-AF949A918467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227D1B8C-88F5-421E-A76A-A3D2069F33E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC7858F6-5E4F-45ED-ADA6-9C1E3287A2F2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="125">
   <si>
     <t>Test Case#</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>1. Vẫn đăng ký thành công</t>
-  </si>
-  <si>
     <t>Đăng ký mà không nhập thông tin</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
   </si>
   <si>
     <t>1.Hiện thị thông báo lỗi "mật khẩu bạn nhập không khớp"</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
   <si>
     <t>Đã đăng ký tài khoản</t>
@@ -411,12 +405,6 @@
   </si>
   <si>
     <t xml:space="preserve">1.Họ tên được cập nhật và hiển thị thông báo thành công
-2.Thông báo lỗi và lỗi validate phần password 
-3.Dữ liệu đã cập nhật trong Database
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Họ tên được cập nhật và hiển thị thông báo thành công
 2.Thông báo chỉnh sửa thành công
 3.Dữ liệu đã cập nhật trong Database.
 </t>
@@ -469,9 +457,6 @@
     <t>1.Email chỉ hiển thị dưới dạng không chỉnh sửa được</t>
   </si>
   <si>
-    <t>1. Vẫn chỉnh sửa được email</t>
-  </si>
-  <si>
     <t>Quay lại trang chủ</t>
   </si>
   <si>
@@ -479,9 +464,6 @@
   </si>
   <si>
     <t>1.Chức vụ chỉ hiển thị dưới dạng không chỉnh sửa được</t>
-  </si>
-  <si>
-    <t>1. Vẫn chỉnh sửa được chức vụ</t>
   </si>
   <si>
     <t>Chức vụ của người dùng chỉ hiển thị, không thể chỉnh sửa</t>
@@ -493,6 +475,19 @@
   </si>
   <si>
     <t>Chức vụ: Admin</t>
+  </si>
+  <si>
+    <t>1. Hiển thị thông báo lỗi email không hợp lệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Họ tên được cập nhật và hiển thị thông báo thành công
+2.Kiểm tra cập nhật trong Database
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Họ tên được cập nhật và hiển thị thông báo thành công
+2.Dữ liệu đã cập nhật trong Database
+</t>
   </si>
 </sst>
 </file>
@@ -607,28 +602,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.89996032593768116"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -646,13 +620,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -660,7 +627,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor theme="3" tint="0.89996032593768116"/>
         </patternFill>
       </fill>
     </dxf>
@@ -996,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FEF34C-D8E2-48D7-991A-F3EAED28713A}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,7 +980,7 @@
     <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1091,13 +1058,13 @@
         <v>21</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
@@ -1105,25 +1072,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>23</v>
@@ -1131,28 +1098,28 @@
     </row>
     <row r="5" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>23</v>
@@ -1160,10 +1127,10 @@
     </row>
     <row r="6" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -1172,16 +1139,16 @@
         <v>19</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="H6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>23</v>
@@ -1189,13 +1156,13 @@
     </row>
     <row r="7" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>19</v>
@@ -1207,10 +1174,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>23</v>
@@ -1218,28 +1185,28 @@
     </row>
     <row r="8" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="E8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>23</v>
@@ -1247,28 +1214,28 @@
     </row>
     <row r="9" spans="1:9" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="H9" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>23</v>
@@ -1276,57 +1243,57 @@
     </row>
     <row r="10" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="E11" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="H11" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>23</v>
@@ -1334,28 +1301,28 @@
     </row>
     <row r="12" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>23</v>
@@ -1363,57 +1330,57 @@
     </row>
     <row r="13" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="G14" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>23</v>
@@ -1421,202 +1388,202 @@
     </row>
     <row r="15" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="B17" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="E17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="B18" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="H18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="I18" s="6" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="H19" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>126</v>
-      </c>
       <c r="G20" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>23</v>
@@ -1627,20 +1594,20 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="G21">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+  <conditionalFormatting sqref="A1:I21">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:I21">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="G21">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>